<commit_message>
Latest code with optimization
</commit_message>
<xml_diff>
--- a/src/Data/NewOrderStandard.xlsx
+++ b/src/Data/NewOrderStandard.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="403">
   <si>
     <t>Product</t>
   </si>
@@ -1615,9 +1615,6 @@
     <t>ashwanis@yopmail.com</t>
   </si>
   <si>
-    <t>E-Signature</t>
-  </si>
-  <si>
     <t>3, Julius-Tandler-Platz, Wien, Austria, Wien, 1090</t>
   </si>
   <si>
@@ -1633,21 +1630,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Hub Product With 5 to 10 Disscount - End to End with Docu-Sign Intergration</t>
-  </si>
-  <si>
-    <t>All Without End to End with Email Intergration</t>
-  </si>
-  <si>
-    <t>Manual Offnet</t>
-  </si>
-  <si>
-    <t>Re val</t>
-  </si>
-  <si>
-    <t>Re nego</t>
-  </si>
-  <si>
     <t>K0120424</t>
   </si>
   <si>
@@ -1655,6 +1637,18 @@
   </si>
   <si>
     <t>Quote Level &gt; Percentage Off</t>
+  </si>
+  <si>
+    <t>Hub Product Without disscount Disscount - End to End with Email Intergration</t>
+  </si>
+  <si>
+    <t>Ethernet P2P Order Without disscount Disscount - End to End with Email Intergration</t>
+  </si>
+  <si>
+    <t>E-Singnature</t>
+  </si>
+  <si>
+    <t>Renegotiate</t>
   </si>
 </sst>
 </file>
@@ -1735,7 +1729,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1804,43 +1798,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1849,7 +1806,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1948,31 +1905,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8002,15 +7958,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF6"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" style="43" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -8042,43 +7998,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
-        <v>395</v>
-      </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
+      <c r="A1" s="45" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="45"/>
+      <c r="AD1" s="45"/>
+      <c r="AE1" s="45"/>
       <c r="AF1" s="45"/>
     </row>
     <row r="2" spans="1:32" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="42" t="s">
         <v>340</v>
       </c>
       <c r="B2" s="35" t="s">
@@ -8172,24 +8128,24 @@
         <v>365</v>
       </c>
       <c r="AF2" s="34" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
+        <v>399</v>
+      </c>
+      <c r="B3" s="44" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
-        <v>397</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>384</v>
-      </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="44" t="s">
         <v>385</v>
       </c>
-      <c r="D3" s="38" t="s">
-        <v>402</v>
-      </c>
-      <c r="E3" s="38">
-        <v>266734</v>
+      <c r="D3" s="44" t="s">
+        <v>396</v>
+      </c>
+      <c r="E3" s="44">
+        <v>267734</v>
       </c>
       <c r="F3" s="36" t="s">
         <v>373</v>
@@ -8197,7 +8153,7 @@
       <c r="G3" s="36"/>
       <c r="H3" s="36"/>
       <c r="I3" s="33" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J3" s="33"/>
       <c r="K3" s="33" t="s">
@@ -8219,40 +8175,40 @@
       <c r="Q3" s="32" t="s">
         <v>369</v>
       </c>
-      <c r="R3" s="38" t="s">
+      <c r="R3" s="44" t="s">
         <v>386</v>
       </c>
-      <c r="S3" s="38" t="s">
+      <c r="S3" s="44" t="s">
         <v>387</v>
       </c>
-      <c r="T3" s="41" t="s">
+      <c r="T3" s="47" t="s">
         <v>388</v>
       </c>
-      <c r="U3" s="38" t="s">
+      <c r="U3" s="44" t="s">
         <v>389</v>
       </c>
-      <c r="V3" s="38">
+      <c r="V3" s="44">
         <v>123566534</v>
       </c>
-      <c r="W3" s="38">
+      <c r="W3" s="44">
         <v>4534534534</v>
       </c>
-      <c r="X3" s="38" t="s">
-        <v>403</v>
-      </c>
-      <c r="Y3" s="38" t="s">
-        <v>404</v>
-      </c>
-      <c r="Z3" s="38">
+      <c r="X3" s="44" t="s">
+        <v>397</v>
+      </c>
+      <c r="Y3" s="44" t="s">
+        <v>398</v>
+      </c>
+      <c r="Z3" s="44">
         <v>3</v>
       </c>
-      <c r="AA3" s="38">
+      <c r="AA3" s="44">
         <v>3</v>
       </c>
-      <c r="AB3" s="38" t="s">
-        <v>396</v>
-      </c>
-      <c r="AC3" s="41" t="s">
+      <c r="AB3" s="44" t="s">
+        <v>395</v>
+      </c>
+      <c r="AC3" s="47" t="s">
         <v>390</v>
       </c>
       <c r="AD3" s="32" t="s">
@@ -8262,22 +8218,22 @@
         <v>371</v>
       </c>
       <c r="AF3" s="32" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
       <c r="F4" s="36" t="s">
         <v>373</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
       <c r="I4" s="33" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J4" s="33"/>
       <c r="K4" s="33" t="s">
@@ -8299,18 +8255,18 @@
       <c r="Q4" s="32" t="s">
         <v>369</v>
       </c>
-      <c r="R4" s="40"/>
-      <c r="S4" s="40"/>
-      <c r="T4" s="46"/>
-      <c r="U4" s="40"/>
-      <c r="V4" s="40"/>
-      <c r="W4" s="40"/>
-      <c r="X4" s="40"/>
-      <c r="Y4" s="40"/>
-      <c r="Z4" s="40"/>
-      <c r="AA4" s="40"/>
-      <c r="AB4" s="39"/>
-      <c r="AC4" s="46"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="44"/>
+      <c r="Y4" s="44"/>
+      <c r="Z4" s="44"/>
+      <c r="AA4" s="44"/>
+      <c r="AB4" s="44"/>
+      <c r="AC4" s="47"/>
       <c r="AD4" s="32" t="s">
         <v>370</v>
       </c>
@@ -8318,24 +8274,24 @@
         <v>371</v>
       </c>
       <c r="AF4" s="32" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
-        <v>398</v>
+        <v>393</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
+        <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="C5" s="38" t="s">
         <v>385</v>
       </c>
-      <c r="D5" s="38">
-        <v>100119208</v>
+      <c r="D5" s="38" t="s">
+        <v>396</v>
       </c>
       <c r="E5" s="38">
-        <v>265341</v>
+        <v>267757</v>
       </c>
       <c r="F5" s="32" t="s">
         <v>347</v>
@@ -8343,10 +8299,10 @@
       <c r="G5" s="32"/>
       <c r="H5" s="32"/>
       <c r="I5" s="33" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K5" s="33" t="s">
         <v>367</v>
@@ -8359,39 +8315,40 @@
         <v>343</v>
       </c>
       <c r="O5" s="32" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="P5" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="39" t="s">
+        <v>386</v>
+      </c>
+      <c r="S5" s="39" t="s">
+        <v>387</v>
+      </c>
+      <c r="T5" s="40" t="s">
+        <v>388</v>
+      </c>
+      <c r="U5" s="39" t="s">
+        <v>389</v>
+      </c>
+      <c r="V5" s="39">
+        <v>123566534</v>
+      </c>
+      <c r="W5" s="39">
+        <v>4534534534</v>
+      </c>
+      <c r="X5" s="39" t="s">
+        <v>397</v>
+      </c>
+      <c r="Y5" s="39"/>
+      <c r="Z5" s="39"/>
+      <c r="AA5" s="39"/>
+      <c r="AB5" s="39" t="s">
         <v>401</v>
       </c>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="38" t="s">
-        <v>386</v>
-      </c>
-      <c r="S5" s="38" t="s">
-        <v>387</v>
-      </c>
-      <c r="T5" s="41" t="s">
-        <v>388</v>
-      </c>
-      <c r="U5" s="38" t="s">
-        <v>389</v>
-      </c>
-      <c r="V5" s="38">
-        <v>123566534</v>
-      </c>
-      <c r="W5" s="38">
-        <v>4534534534</v>
-      </c>
-      <c r="X5" s="38">
-        <v>10000</v>
-      </c>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="38" t="s">
-        <v>391</v>
-      </c>
-      <c r="AC5" s="41" t="s">
+      <c r="AC5" s="40" t="s">
         <v>390</v>
       </c>
       <c r="AD5" s="32" t="s">
@@ -8400,108 +8357,41 @@
       <c r="AE5" s="32" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="32" t="s">
-        <v>347</v>
-      </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="33" t="s">
-        <v>392</v>
-      </c>
-      <c r="J6" s="33" t="s">
-        <v>392</v>
-      </c>
-      <c r="K6" s="33" t="s">
-        <v>367</v>
-      </c>
-      <c r="L6" s="33"/>
-      <c r="M6" s="32" t="s">
-        <v>342</v>
-      </c>
-      <c r="N6" s="32" t="s">
-        <v>343</v>
-      </c>
-      <c r="O6" s="32" t="s">
-        <v>399</v>
-      </c>
-      <c r="P6" s="32" t="s">
-        <v>399</v>
-      </c>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="39"/>
-      <c r="V6" s="39"/>
-      <c r="W6" s="39"/>
-      <c r="X6" s="39"/>
-      <c r="Y6" s="39"/>
-      <c r="Z6" s="39"/>
-      <c r="AA6" s="39"/>
-      <c r="AC6" s="42"/>
-      <c r="AD6" s="32" t="s">
-        <v>370</v>
-      </c>
-      <c r="AE6" s="32" t="s">
-        <v>371</v>
+      <c r="AF5" s="32" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="U3:U4"/>
+  <mergeCells count="18">
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="W3:W4"/>
     <mergeCell ref="X3:X4"/>
     <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="T3:T4"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="X5:X6"/>
-    <mergeCell ref="Y5:Y6"/>
-    <mergeCell ref="Z5:Z6"/>
-    <mergeCell ref="AA5:AA6"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="U3:U4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="T5" r:id="rId1"/>
     <hyperlink ref="AC5" r:id="rId2"/>
-    <hyperlink ref="T6" r:id="rId3" display="Ashwani.singh31@colt.net"/>
-    <hyperlink ref="AC6" r:id="rId4" display="ashwanis@yopmail.com"/>
-    <hyperlink ref="T3" r:id="rId5"/>
-    <hyperlink ref="AC3" r:id="rId6"/>
+    <hyperlink ref="T3" r:id="rId3"/>
+    <hyperlink ref="AC3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId5"/>
   <customProperties>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId8"/>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId6"/>
   </customProperties>
 </worksheet>
 </file>
@@ -13674,19 +13564,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1101" r:id="rId463" name="Control 77">
+        <control shapeId="1025" r:id="rId463" name="Control 1">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>156</xdr:row>
+                <xdr:row>1</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>156</xdr:row>
+                <xdr:row>1</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -13694,24 +13584,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1101" r:id="rId463" name="Control 77"/>
+        <control shapeId="1025" r:id="rId463" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1100" r:id="rId465" name="Control 76">
+        <control shapeId="1026" r:id="rId465" name="Control 2">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>153</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>153</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -13719,24 +13609,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1100" r:id="rId465" name="Control 76"/>
+        <control shapeId="1026" r:id="rId465" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1099" r:id="rId466" name="Control 75">
+        <control shapeId="1027" r:id="rId466" name="Control 3">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>150</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>150</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -13744,24 +13634,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1099" r:id="rId466" name="Control 75"/>
+        <control shapeId="1027" r:id="rId466" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1098" r:id="rId467" name="Control 74">
+        <control shapeId="1028" r:id="rId467" name="Control 4">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>148</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>148</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -13769,24 +13659,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1098" r:id="rId467" name="Control 74"/>
+        <control shapeId="1028" r:id="rId467" name="Control 4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1097" r:id="rId468" name="Control 73">
+        <control shapeId="1029" r:id="rId468" name="Control 5">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>146</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>146</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -13794,24 +13684,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1097" r:id="rId468" name="Control 73"/>
+        <control shapeId="1029" r:id="rId468" name="Control 5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1096" r:id="rId469" name="Control 72">
+        <control shapeId="1030" r:id="rId469" name="Control 6">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>144</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>144</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -13819,24 +13709,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1096" r:id="rId469" name="Control 72"/>
+        <control shapeId="1030" r:id="rId469" name="Control 6"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1095" r:id="rId470" name="Control 71">
+        <control shapeId="1031" r:id="rId470" name="Control 7">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>142</xdr:row>
+                <xdr:row>7</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>142</xdr:row>
+                <xdr:row>7</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -13844,24 +13734,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1095" r:id="rId470" name="Control 71"/>
+        <control shapeId="1031" r:id="rId470" name="Control 7"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1094" r:id="rId471" name="Control 70">
+        <control shapeId="1032" r:id="rId471" name="Control 8">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>140</xdr:row>
+                <xdr:row>8</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>140</xdr:row>
+                <xdr:row>8</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -13869,24 +13759,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1094" r:id="rId471" name="Control 70"/>
+        <control shapeId="1032" r:id="rId471" name="Control 8"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1093" r:id="rId472" name="Control 69">
+        <control shapeId="1033" r:id="rId472" name="Control 9">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>138</xdr:row>
+                <xdr:row>12</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>138</xdr:row>
+                <xdr:row>12</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -13894,24 +13784,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1093" r:id="rId472" name="Control 69"/>
+        <control shapeId="1033" r:id="rId472" name="Control 9"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1092" r:id="rId473" name="Control 68">
+        <control shapeId="1034" r:id="rId473" name="Control 10">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>136</xdr:row>
+                <xdr:row>14</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>136</xdr:row>
+                <xdr:row>14</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -13919,24 +13809,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1092" r:id="rId473" name="Control 68"/>
+        <control shapeId="1034" r:id="rId473" name="Control 10"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1091" r:id="rId474" name="Control 67">
+        <control shapeId="1035" r:id="rId474" name="Control 11">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>133</xdr:row>
+                <xdr:row>15</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>133</xdr:row>
+                <xdr:row>15</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -13944,24 +13834,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1091" r:id="rId474" name="Control 67"/>
+        <control shapeId="1035" r:id="rId474" name="Control 11"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1090" r:id="rId475" name="Control 66">
+        <control shapeId="1036" r:id="rId475" name="Control 12">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>131</xdr:row>
+                <xdr:row>17</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>131</xdr:row>
+                <xdr:row>17</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -13969,24 +13859,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1090" r:id="rId475" name="Control 66"/>
+        <control shapeId="1036" r:id="rId475" name="Control 12"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1089" r:id="rId476" name="Control 65">
+        <control shapeId="1037" r:id="rId476" name="Control 13">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>129</xdr:row>
+                <xdr:row>19</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>129</xdr:row>
+                <xdr:row>19</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -13994,24 +13884,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1089" r:id="rId476" name="Control 65"/>
+        <control shapeId="1037" r:id="rId476" name="Control 13"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1088" r:id="rId477" name="Control 64">
+        <control shapeId="1038" r:id="rId477" name="Control 14">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>127</xdr:row>
+                <xdr:row>21</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>127</xdr:row>
+                <xdr:row>21</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14019,24 +13909,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1088" r:id="rId477" name="Control 64"/>
+        <control shapeId="1038" r:id="rId477" name="Control 14"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1087" r:id="rId478" name="Control 63">
+        <control shapeId="1039" r:id="rId478" name="Control 15">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>125</xdr:row>
+                <xdr:row>22</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>125</xdr:row>
+                <xdr:row>22</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14044,24 +13934,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1087" r:id="rId478" name="Control 63"/>
+        <control shapeId="1039" r:id="rId478" name="Control 15"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1086" r:id="rId479" name="Control 62">
+        <control shapeId="1040" r:id="rId479" name="Control 16">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>119</xdr:row>
+                <xdr:row>26</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>119</xdr:row>
+                <xdr:row>26</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14069,24 +13959,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1086" r:id="rId479" name="Control 62"/>
+        <control shapeId="1040" r:id="rId479" name="Control 16"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1085" r:id="rId480" name="Control 61">
+        <control shapeId="1041" r:id="rId480" name="Control 17">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>117</xdr:row>
+                <xdr:row>29</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>117</xdr:row>
+                <xdr:row>29</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14094,24 +13984,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1085" r:id="rId480" name="Control 61"/>
+        <control shapeId="1041" r:id="rId480" name="Control 17"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1084" r:id="rId481" name="Control 60">
+        <control shapeId="1042" r:id="rId481" name="Control 18">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>111</xdr:row>
+                <xdr:row>30</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>111</xdr:row>
+                <xdr:row>30</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14119,24 +14009,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1084" r:id="rId481" name="Control 60"/>
+        <control shapeId="1042" r:id="rId481" name="Control 18"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1083" r:id="rId482" name="Control 59">
+        <control shapeId="1043" r:id="rId482" name="Control 19">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>107</xdr:row>
+                <xdr:row>31</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>107</xdr:row>
+                <xdr:row>31</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14144,24 +14034,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1083" r:id="rId482" name="Control 59"/>
+        <control shapeId="1043" r:id="rId482" name="Control 19"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1082" r:id="rId483" name="Control 58">
+        <control shapeId="1044" r:id="rId483" name="Control 20">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>105</xdr:row>
+                <xdr:row>32</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>105</xdr:row>
+                <xdr:row>32</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14169,24 +14059,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1082" r:id="rId483" name="Control 58"/>
+        <control shapeId="1044" r:id="rId483" name="Control 20"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1081" r:id="rId484" name="Control 57">
+        <control shapeId="1045" r:id="rId484" name="Control 21">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>103</xdr:row>
+                <xdr:row>33</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>103</xdr:row>
+                <xdr:row>33</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14194,24 +14084,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1081" r:id="rId484" name="Control 57"/>
+        <control shapeId="1045" r:id="rId484" name="Control 21"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1080" r:id="rId485" name="Control 56">
+        <control shapeId="1046" r:id="rId485" name="Control 22">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>101</xdr:row>
+                <xdr:row>34</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>101</xdr:row>
+                <xdr:row>34</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14219,24 +14109,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1080" r:id="rId485" name="Control 56"/>
+        <control shapeId="1046" r:id="rId485" name="Control 22"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1079" r:id="rId486" name="Control 55">
+        <control shapeId="1047" r:id="rId486" name="Control 23">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>100</xdr:row>
+                <xdr:row>35</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>100</xdr:row>
+                <xdr:row>35</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14244,24 +14134,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1079" r:id="rId486" name="Control 55"/>
+        <control shapeId="1047" r:id="rId486" name="Control 23"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1078" r:id="rId487" name="Control 54">
+        <control shapeId="1048" r:id="rId487" name="Control 24">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>97</xdr:row>
+                <xdr:row>36</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>97</xdr:row>
+                <xdr:row>36</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14269,24 +14159,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1078" r:id="rId487" name="Control 54"/>
+        <control shapeId="1048" r:id="rId487" name="Control 24"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1077" r:id="rId488" name="Control 53">
+        <control shapeId="1049" r:id="rId488" name="Control 25">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>90</xdr:row>
+                <xdr:row>37</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>90</xdr:row>
+                <xdr:row>37</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14294,24 +14184,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1077" r:id="rId488" name="Control 53"/>
+        <control shapeId="1049" r:id="rId488" name="Control 25"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1076" r:id="rId489" name="Control 52">
+        <control shapeId="1050" r:id="rId489" name="Control 26">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>89</xdr:row>
+                <xdr:row>41</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>89</xdr:row>
+                <xdr:row>41</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14319,24 +14209,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1076" r:id="rId489" name="Control 52"/>
+        <control shapeId="1050" r:id="rId489" name="Control 26"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1075" r:id="rId490" name="Control 51">
+        <control shapeId="1051" r:id="rId490" name="Control 27">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>87</xdr:row>
+                <xdr:row>43</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>87</xdr:row>
+                <xdr:row>43</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14344,24 +14234,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1075" r:id="rId490" name="Control 51"/>
+        <control shapeId="1051" r:id="rId490" name="Control 27"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1074" r:id="rId491" name="Control 50">
+        <control shapeId="1052" r:id="rId491" name="Control 28">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>86</xdr:row>
+                <xdr:row>45</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>86</xdr:row>
+                <xdr:row>45</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14369,24 +14259,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1074" r:id="rId491" name="Control 50"/>
+        <control shapeId="1052" r:id="rId491" name="Control 28"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1073" r:id="rId492" name="Control 49">
+        <control shapeId="1053" r:id="rId492" name="Control 29">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>85</xdr:row>
+                <xdr:row>46</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>85</xdr:row>
+                <xdr:row>46</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14394,24 +14284,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1073" r:id="rId492" name="Control 49"/>
+        <control shapeId="1053" r:id="rId492" name="Control 29"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1072" r:id="rId493" name="Control 48">
+        <control shapeId="1054" r:id="rId493" name="Control 30">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>82</xdr:row>
+                <xdr:row>50</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>82</xdr:row>
+                <xdr:row>50</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14419,24 +14309,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1072" r:id="rId493" name="Control 48"/>
+        <control shapeId="1054" r:id="rId493" name="Control 30"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1071" r:id="rId494" name="Control 47">
+        <control shapeId="1055" r:id="rId494" name="Control 31">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>81</xdr:row>
+                <xdr:row>51</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>81</xdr:row>
+                <xdr:row>51</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14444,24 +14334,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1071" r:id="rId494" name="Control 47"/>
+        <control shapeId="1055" r:id="rId494" name="Control 31"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1070" r:id="rId495" name="Control 46">
+        <control shapeId="1056" r:id="rId495" name="Control 32">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>80</xdr:row>
+                <xdr:row>53</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>80</xdr:row>
+                <xdr:row>53</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14469,24 +14359,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1070" r:id="rId495" name="Control 46"/>
+        <control shapeId="1056" r:id="rId495" name="Control 32"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1069" r:id="rId496" name="Control 45">
+        <control shapeId="1057" r:id="rId496" name="Control 33">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>76</xdr:row>
+                <xdr:row>54</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>76</xdr:row>
+                <xdr:row>54</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14494,24 +14384,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1069" r:id="rId496" name="Control 45"/>
+        <control shapeId="1057" r:id="rId496" name="Control 33"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1068" r:id="rId497" name="Control 44">
+        <control shapeId="1058" r:id="rId497" name="Control 34">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>74</xdr:row>
+                <xdr:row>56</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>74</xdr:row>
+                <xdr:row>56</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14519,24 +14409,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1068" r:id="rId497" name="Control 44"/>
+        <control shapeId="1058" r:id="rId497" name="Control 34"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1067" r:id="rId498" name="Control 43">
+        <control shapeId="1059" r:id="rId498" name="Control 35">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>73</xdr:row>
+                <xdr:row>59</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>73</xdr:row>
+                <xdr:row>59</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14544,24 +14434,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1067" r:id="rId498" name="Control 43"/>
+        <control shapeId="1059" r:id="rId498" name="Control 35"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1066" r:id="rId499" name="Control 42">
+        <control shapeId="1060" r:id="rId499" name="Control 36">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>71</xdr:row>
+                <xdr:row>62</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>71</xdr:row>
+                <xdr:row>62</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14569,24 +14459,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1066" r:id="rId499" name="Control 42"/>
+        <control shapeId="1060" r:id="rId499" name="Control 36"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1065" r:id="rId500" name="Control 41">
+        <control shapeId="1061" r:id="rId500" name="Control 37">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>70</xdr:row>
+                <xdr:row>63</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>70</xdr:row>
+                <xdr:row>63</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14594,24 +14484,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1065" r:id="rId500" name="Control 41"/>
+        <control shapeId="1061" r:id="rId500" name="Control 37"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1064" r:id="rId501" name="Control 40">
+        <control shapeId="1062" r:id="rId501" name="Control 38">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>69</xdr:row>
+                <xdr:row>64</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>69</xdr:row>
+                <xdr:row>64</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14619,7 +14509,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1064" r:id="rId501" name="Control 40"/>
+        <control shapeId="1062" r:id="rId501" name="Control 38"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -14649,19 +14539,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1062" r:id="rId503" name="Control 38">
+        <control shapeId="1064" r:id="rId503" name="Control 40">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>64</xdr:row>
+                <xdr:row>69</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>64</xdr:row>
+                <xdr:row>69</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14669,24 +14559,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1062" r:id="rId503" name="Control 38"/>
+        <control shapeId="1064" r:id="rId503" name="Control 40"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1061" r:id="rId504" name="Control 37">
+        <control shapeId="1065" r:id="rId504" name="Control 41">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>63</xdr:row>
+                <xdr:row>70</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>63</xdr:row>
+                <xdr:row>70</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14694,24 +14584,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1061" r:id="rId504" name="Control 37"/>
+        <control shapeId="1065" r:id="rId504" name="Control 41"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1060" r:id="rId505" name="Control 36">
+        <control shapeId="1066" r:id="rId505" name="Control 42">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>62</xdr:row>
+                <xdr:row>71</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>62</xdr:row>
+                <xdr:row>71</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14719,24 +14609,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1060" r:id="rId505" name="Control 36"/>
+        <control shapeId="1066" r:id="rId505" name="Control 42"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1059" r:id="rId506" name="Control 35">
+        <control shapeId="1067" r:id="rId506" name="Control 43">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>59</xdr:row>
+                <xdr:row>73</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>59</xdr:row>
+                <xdr:row>73</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14744,24 +14634,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1059" r:id="rId506" name="Control 35"/>
+        <control shapeId="1067" r:id="rId506" name="Control 43"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1058" r:id="rId507" name="Control 34">
+        <control shapeId="1068" r:id="rId507" name="Control 44">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>56</xdr:row>
+                <xdr:row>74</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>56</xdr:row>
+                <xdr:row>74</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14769,24 +14659,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1058" r:id="rId507" name="Control 34"/>
+        <control shapeId="1068" r:id="rId507" name="Control 44"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1057" r:id="rId508" name="Control 33">
+        <control shapeId="1069" r:id="rId508" name="Control 45">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>54</xdr:row>
+                <xdr:row>76</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>54</xdr:row>
+                <xdr:row>76</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14794,24 +14684,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1057" r:id="rId508" name="Control 33"/>
+        <control shapeId="1069" r:id="rId508" name="Control 45"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1056" r:id="rId509" name="Control 32">
+        <control shapeId="1070" r:id="rId509" name="Control 46">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>53</xdr:row>
+                <xdr:row>80</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>53</xdr:row>
+                <xdr:row>80</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14819,24 +14709,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1056" r:id="rId509" name="Control 32"/>
+        <control shapeId="1070" r:id="rId509" name="Control 46"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1055" r:id="rId510" name="Control 31">
+        <control shapeId="1071" r:id="rId510" name="Control 47">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>51</xdr:row>
+                <xdr:row>81</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>51</xdr:row>
+                <xdr:row>81</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14844,24 +14734,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1055" r:id="rId510" name="Control 31"/>
+        <control shapeId="1071" r:id="rId510" name="Control 47"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1054" r:id="rId511" name="Control 30">
+        <control shapeId="1072" r:id="rId511" name="Control 48">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>50</xdr:row>
+                <xdr:row>82</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>50</xdr:row>
+                <xdr:row>82</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14869,24 +14759,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1054" r:id="rId511" name="Control 30"/>
+        <control shapeId="1072" r:id="rId511" name="Control 48"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1053" r:id="rId512" name="Control 29">
+        <control shapeId="1073" r:id="rId512" name="Control 49">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>46</xdr:row>
+                <xdr:row>85</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>46</xdr:row>
+                <xdr:row>85</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14894,24 +14784,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1053" r:id="rId512" name="Control 29"/>
+        <control shapeId="1073" r:id="rId512" name="Control 49"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1052" r:id="rId513" name="Control 28">
+        <control shapeId="1074" r:id="rId513" name="Control 50">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>45</xdr:row>
+                <xdr:row>86</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>45</xdr:row>
+                <xdr:row>86</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14919,24 +14809,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1052" r:id="rId513" name="Control 28"/>
+        <control shapeId="1074" r:id="rId513" name="Control 50"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1051" r:id="rId514" name="Control 27">
+        <control shapeId="1075" r:id="rId514" name="Control 51">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>43</xdr:row>
+                <xdr:row>87</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>43</xdr:row>
+                <xdr:row>87</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14944,24 +14834,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1051" r:id="rId514" name="Control 27"/>
+        <control shapeId="1075" r:id="rId514" name="Control 51"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1050" r:id="rId515" name="Control 26">
+        <control shapeId="1076" r:id="rId515" name="Control 52">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>41</xdr:row>
+                <xdr:row>89</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>41</xdr:row>
+                <xdr:row>89</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14969,24 +14859,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1050" r:id="rId515" name="Control 26"/>
+        <control shapeId="1076" r:id="rId515" name="Control 52"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1049" r:id="rId516" name="Control 25">
+        <control shapeId="1077" r:id="rId516" name="Control 53">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>37</xdr:row>
+                <xdr:row>90</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>37</xdr:row>
+                <xdr:row>90</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -14994,24 +14884,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1049" r:id="rId516" name="Control 25"/>
+        <control shapeId="1077" r:id="rId516" name="Control 53"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1048" r:id="rId517" name="Control 24">
+        <control shapeId="1078" r:id="rId517" name="Control 54">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>36</xdr:row>
+                <xdr:row>97</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>36</xdr:row>
+                <xdr:row>97</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15019,24 +14909,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1048" r:id="rId517" name="Control 24"/>
+        <control shapeId="1078" r:id="rId517" name="Control 54"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1047" r:id="rId518" name="Control 23">
+        <control shapeId="1079" r:id="rId518" name="Control 55">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>35</xdr:row>
+                <xdr:row>100</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>35</xdr:row>
+                <xdr:row>100</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15044,24 +14934,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1047" r:id="rId518" name="Control 23"/>
+        <control shapeId="1079" r:id="rId518" name="Control 55"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1046" r:id="rId519" name="Control 22">
+        <control shapeId="1080" r:id="rId519" name="Control 56">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>34</xdr:row>
+                <xdr:row>101</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>34</xdr:row>
+                <xdr:row>101</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15069,24 +14959,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1046" r:id="rId519" name="Control 22"/>
+        <control shapeId="1080" r:id="rId519" name="Control 56"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1045" r:id="rId520" name="Control 21">
+        <control shapeId="1081" r:id="rId520" name="Control 57">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>33</xdr:row>
+                <xdr:row>103</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>33</xdr:row>
+                <xdr:row>103</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15094,24 +14984,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1045" r:id="rId520" name="Control 21"/>
+        <control shapeId="1081" r:id="rId520" name="Control 57"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1044" r:id="rId521" name="Control 20">
+        <control shapeId="1082" r:id="rId521" name="Control 58">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>32</xdr:row>
+                <xdr:row>105</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>32</xdr:row>
+                <xdr:row>105</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15119,24 +15009,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1044" r:id="rId521" name="Control 20"/>
+        <control shapeId="1082" r:id="rId521" name="Control 58"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1043" r:id="rId522" name="Control 19">
+        <control shapeId="1083" r:id="rId522" name="Control 59">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>31</xdr:row>
+                <xdr:row>107</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>31</xdr:row>
+                <xdr:row>107</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15144,24 +15034,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1043" r:id="rId522" name="Control 19"/>
+        <control shapeId="1083" r:id="rId522" name="Control 59"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1042" r:id="rId523" name="Control 18">
+        <control shapeId="1084" r:id="rId523" name="Control 60">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>30</xdr:row>
+                <xdr:row>111</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>30</xdr:row>
+                <xdr:row>111</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15169,24 +15059,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1042" r:id="rId523" name="Control 18"/>
+        <control shapeId="1084" r:id="rId523" name="Control 60"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1041" r:id="rId524" name="Control 17">
+        <control shapeId="1085" r:id="rId524" name="Control 61">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>29</xdr:row>
+                <xdr:row>117</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>29</xdr:row>
+                <xdr:row>117</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15194,24 +15084,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1041" r:id="rId524" name="Control 17"/>
+        <control shapeId="1085" r:id="rId524" name="Control 61"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1040" r:id="rId525" name="Control 16">
+        <control shapeId="1086" r:id="rId525" name="Control 62">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
+                <xdr:row>119</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
+                <xdr:row>119</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15219,24 +15109,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1040" r:id="rId525" name="Control 16"/>
+        <control shapeId="1086" r:id="rId525" name="Control 62"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1039" r:id="rId526" name="Control 15">
+        <control shapeId="1087" r:id="rId526" name="Control 63">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>22</xdr:row>
+                <xdr:row>125</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>22</xdr:row>
+                <xdr:row>125</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15244,24 +15134,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1039" r:id="rId526" name="Control 15"/>
+        <control shapeId="1087" r:id="rId526" name="Control 63"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1038" r:id="rId527" name="Control 14">
+        <control shapeId="1088" r:id="rId527" name="Control 64">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>21</xdr:row>
+                <xdr:row>127</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>21</xdr:row>
+                <xdr:row>127</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15269,24 +15159,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1038" r:id="rId527" name="Control 14"/>
+        <control shapeId="1088" r:id="rId527" name="Control 64"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1037" r:id="rId528" name="Control 13">
+        <control shapeId="1089" r:id="rId528" name="Control 65">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>19</xdr:row>
+                <xdr:row>129</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>19</xdr:row>
+                <xdr:row>129</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15294,24 +15184,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1037" r:id="rId528" name="Control 13"/>
+        <control shapeId="1089" r:id="rId528" name="Control 65"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId529" name="Control 12">
+        <control shapeId="1090" r:id="rId529" name="Control 66">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>17</xdr:row>
+                <xdr:row>131</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>17</xdr:row>
+                <xdr:row>131</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15319,24 +15209,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1036" r:id="rId529" name="Control 12"/>
+        <control shapeId="1090" r:id="rId529" name="Control 66"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId530" name="Control 11">
+        <control shapeId="1091" r:id="rId530" name="Control 67">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>133</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>133</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15344,24 +15234,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1035" r:id="rId530" name="Control 11"/>
+        <control shapeId="1091" r:id="rId530" name="Control 67"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1034" r:id="rId531" name="Control 10">
+        <control shapeId="1092" r:id="rId531" name="Control 68">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>14</xdr:row>
+                <xdr:row>136</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>14</xdr:row>
+                <xdr:row>136</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15369,24 +15259,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1034" r:id="rId531" name="Control 10"/>
+        <control shapeId="1092" r:id="rId531" name="Control 68"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId532" name="Control 9">
+        <control shapeId="1093" r:id="rId532" name="Control 69">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
+                <xdr:row>138</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>12</xdr:row>
+                <xdr:row>138</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15394,24 +15284,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1033" r:id="rId532" name="Control 9"/>
+        <control shapeId="1093" r:id="rId532" name="Control 69"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId533" name="Control 8">
+        <control shapeId="1094" r:id="rId533" name="Control 70">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>8</xdr:row>
+                <xdr:row>140</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>8</xdr:row>
+                <xdr:row>140</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15419,24 +15309,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1032" r:id="rId533" name="Control 8"/>
+        <control shapeId="1094" r:id="rId533" name="Control 70"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1031" r:id="rId534" name="Control 7">
+        <control shapeId="1095" r:id="rId534" name="Control 71">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>7</xdr:row>
+                <xdr:row>142</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>7</xdr:row>
+                <xdr:row>142</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15444,24 +15334,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1031" r:id="rId534" name="Control 7"/>
+        <control shapeId="1095" r:id="rId534" name="Control 71"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId535" name="Control 6">
+        <control shapeId="1096" r:id="rId535" name="Control 72">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:row>144</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:row>144</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15469,24 +15359,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1030" r:id="rId535" name="Control 6"/>
+        <control shapeId="1096" r:id="rId535" name="Control 72"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId536" name="Control 5">
+        <control shapeId="1097" r:id="rId536" name="Control 73">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>146</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>146</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15494,24 +15384,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId536" name="Control 5"/>
+        <control shapeId="1097" r:id="rId536" name="Control 73"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId537" name="Control 4">
+        <control shapeId="1098" r:id="rId537" name="Control 74">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>148</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>148</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15519,24 +15409,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId537" name="Control 4"/>
+        <control shapeId="1098" r:id="rId537" name="Control 74"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId538" name="Control 3">
+        <control shapeId="1099" r:id="rId538" name="Control 75">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>150</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>150</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15544,24 +15434,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId538" name="Control 3"/>
+        <control shapeId="1099" r:id="rId538" name="Control 75"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId539" name="Control 2">
+        <control shapeId="1100" r:id="rId539" name="Control 76">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>153</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>153</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15569,24 +15459,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId539" name="Control 2"/>
+        <control shapeId="1100" r:id="rId539" name="Control 76"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId540" name="Control 1">
+        <control shapeId="1101" r:id="rId540" name="Control 77">
           <controlPr defaultSize="0" r:id="rId464">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
+                <xdr:row>156</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>1</xdr:row>
+                <xdr:row>156</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -15594,7 +15484,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId540" name="Control 1"/>
+        <control shapeId="1101" r:id="rId540" name="Control 77"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -17928,19 +17818,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2083" r:id="rId183" name="Control 35">
+        <control shapeId="2049" r:id="rId183" name="Control 1">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>72</xdr:row>
+                <xdr:row>1</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>72</xdr:row>
+                <xdr:row>1</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -17948,24 +17838,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2083" r:id="rId183" name="Control 35"/>
+        <control shapeId="2049" r:id="rId183" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2082" r:id="rId185" name="Control 34">
+        <control shapeId="2050" r:id="rId185" name="Control 2">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>69</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>69</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -17973,24 +17863,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2082" r:id="rId185" name="Control 34"/>
+        <control shapeId="2050" r:id="rId185" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2081" r:id="rId186" name="Control 33">
+        <control shapeId="2051" r:id="rId186" name="Control 3">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>66</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>66</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -17998,24 +17888,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2081" r:id="rId186" name="Control 33"/>
+        <control shapeId="2051" r:id="rId186" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2080" r:id="rId187" name="Control 32">
+        <control shapeId="2052" r:id="rId187" name="Control 4">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>64</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>64</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18023,24 +17913,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2080" r:id="rId187" name="Control 32"/>
+        <control shapeId="2052" r:id="rId187" name="Control 4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2079" r:id="rId188" name="Control 31">
+        <control shapeId="2053" r:id="rId188" name="Control 5">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>61</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>61</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18048,24 +17938,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2079" r:id="rId188" name="Control 31"/>
+        <control shapeId="2053" r:id="rId188" name="Control 5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2078" r:id="rId189" name="Control 30">
+        <control shapeId="2054" r:id="rId189" name="Control 6">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>60</xdr:row>
+                <xdr:row>7</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>60</xdr:row>
+                <xdr:row>7</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18073,24 +17963,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2078" r:id="rId189" name="Control 30"/>
+        <control shapeId="2054" r:id="rId189" name="Control 6"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2077" r:id="rId190" name="Control 29">
+        <control shapeId="2055" r:id="rId190" name="Control 7">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>58</xdr:row>
+                <xdr:row>11</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>58</xdr:row>
+                <xdr:row>11</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18098,24 +17988,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2077" r:id="rId190" name="Control 29"/>
+        <control shapeId="2055" r:id="rId190" name="Control 7"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2076" r:id="rId191" name="Control 28">
+        <control shapeId="2056" r:id="rId191" name="Control 8">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>56</xdr:row>
+                <xdr:row>13</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>56</xdr:row>
+                <xdr:row>13</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18123,24 +18013,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2076" r:id="rId191" name="Control 28"/>
+        <control shapeId="2056" r:id="rId191" name="Control 8"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2075" r:id="rId192" name="Control 27">
+        <control shapeId="2057" r:id="rId192" name="Control 9">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>52</xdr:row>
+                <xdr:row>15</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>52</xdr:row>
+                <xdr:row>15</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18148,24 +18038,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2075" r:id="rId192" name="Control 27"/>
+        <control shapeId="2057" r:id="rId192" name="Control 9"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2074" r:id="rId193" name="Control 26">
+        <control shapeId="2058" r:id="rId193" name="Control 10">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>49</xdr:row>
+                <xdr:row>17</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>49</xdr:row>
+                <xdr:row>17</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18173,24 +18063,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2074" r:id="rId193" name="Control 26"/>
+        <control shapeId="2058" r:id="rId193" name="Control 10"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2073" r:id="rId194" name="Control 25">
+        <control shapeId="2059" r:id="rId194" name="Control 11">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>46</xdr:row>
+                <xdr:row>19</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>46</xdr:row>
+                <xdr:row>19</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18198,24 +18088,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2073" r:id="rId194" name="Control 25"/>
+        <control shapeId="2059" r:id="rId194" name="Control 11"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2072" r:id="rId195" name="Control 24">
+        <control shapeId="2060" r:id="rId195" name="Control 12">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>44</xdr:row>
+                <xdr:row>21</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>44</xdr:row>
+                <xdr:row>21</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18223,24 +18113,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2072" r:id="rId195" name="Control 24"/>
+        <control shapeId="2060" r:id="rId195" name="Control 12"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2071" r:id="rId196" name="Control 23">
+        <control shapeId="2061" r:id="rId196" name="Control 13">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>43</xdr:row>
+                <xdr:row>23</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>43</xdr:row>
+                <xdr:row>23</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18248,24 +18138,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2071" r:id="rId196" name="Control 23"/>
+        <control shapeId="2061" r:id="rId196" name="Control 13"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2070" r:id="rId197" name="Control 22">
+        <control shapeId="2062" r:id="rId197" name="Control 14">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>41</xdr:row>
+                <xdr:row>25</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>41</xdr:row>
+                <xdr:row>25</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18273,24 +18163,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2070" r:id="rId197" name="Control 22"/>
+        <control shapeId="2062" r:id="rId197" name="Control 14"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2069" r:id="rId198" name="Control 21">
+        <control shapeId="2063" r:id="rId198" name="Control 15">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>40</xdr:row>
+                <xdr:row>26</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>40</xdr:row>
+                <xdr:row>26</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18298,24 +18188,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2069" r:id="rId198" name="Control 21"/>
+        <control shapeId="2063" r:id="rId198" name="Control 15"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2068" r:id="rId199" name="Control 20">
+        <control shapeId="2064" r:id="rId199" name="Control 16">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>37</xdr:row>
+                <xdr:row>27</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>37</xdr:row>
+                <xdr:row>27</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18323,24 +18213,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2068" r:id="rId199" name="Control 20"/>
+        <control shapeId="2064" r:id="rId199" name="Control 16"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2067" r:id="rId200" name="Control 19">
+        <control shapeId="2065" r:id="rId200" name="Control 17">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>35</xdr:row>
+                <xdr:row>29</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>35</xdr:row>
+                <xdr:row>29</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18348,7 +18238,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2067" r:id="rId200" name="Control 19"/>
+        <control shapeId="2065" r:id="rId200" name="Control 17"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -18378,19 +18268,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2065" r:id="rId202" name="Control 17">
+        <control shapeId="2067" r:id="rId202" name="Control 19">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>29</xdr:row>
+                <xdr:row>35</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>29</xdr:row>
+                <xdr:row>35</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18398,24 +18288,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2065" r:id="rId202" name="Control 17"/>
+        <control shapeId="2067" r:id="rId202" name="Control 19"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2064" r:id="rId203" name="Control 16">
+        <control shapeId="2068" r:id="rId203" name="Control 20">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>27</xdr:row>
+                <xdr:row>37</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>27</xdr:row>
+                <xdr:row>37</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18423,24 +18313,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2064" r:id="rId203" name="Control 16"/>
+        <control shapeId="2068" r:id="rId203" name="Control 20"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2063" r:id="rId204" name="Control 15">
+        <control shapeId="2069" r:id="rId204" name="Control 21">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
+                <xdr:row>40</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
+                <xdr:row>40</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18448,24 +18338,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2063" r:id="rId204" name="Control 15"/>
+        <control shapeId="2069" r:id="rId204" name="Control 21"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2062" r:id="rId205" name="Control 14">
+        <control shapeId="2070" r:id="rId205" name="Control 22">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>25</xdr:row>
+                <xdr:row>41</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>25</xdr:row>
+                <xdr:row>41</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18473,24 +18363,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2062" r:id="rId205" name="Control 14"/>
+        <control shapeId="2070" r:id="rId205" name="Control 22"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2061" r:id="rId206" name="Control 13">
+        <control shapeId="2071" r:id="rId206" name="Control 23">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>23</xdr:row>
+                <xdr:row>43</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>23</xdr:row>
+                <xdr:row>43</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18498,24 +18388,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2061" r:id="rId206" name="Control 13"/>
+        <control shapeId="2071" r:id="rId206" name="Control 23"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2060" r:id="rId207" name="Control 12">
+        <control shapeId="2072" r:id="rId207" name="Control 24">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>21</xdr:row>
+                <xdr:row>44</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>21</xdr:row>
+                <xdr:row>44</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18523,24 +18413,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2060" r:id="rId207" name="Control 12"/>
+        <control shapeId="2072" r:id="rId207" name="Control 24"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2059" r:id="rId208" name="Control 11">
+        <control shapeId="2073" r:id="rId208" name="Control 25">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>19</xdr:row>
+                <xdr:row>46</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>19</xdr:row>
+                <xdr:row>46</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18548,24 +18438,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2059" r:id="rId208" name="Control 11"/>
+        <control shapeId="2073" r:id="rId208" name="Control 25"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2058" r:id="rId209" name="Control 10">
+        <control shapeId="2074" r:id="rId209" name="Control 26">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>17</xdr:row>
+                <xdr:row>49</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>17</xdr:row>
+                <xdr:row>49</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18573,24 +18463,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2058" r:id="rId209" name="Control 10"/>
+        <control shapeId="2074" r:id="rId209" name="Control 26"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2057" r:id="rId210" name="Control 9">
+        <control shapeId="2075" r:id="rId210" name="Control 27">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>52</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>52</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18598,24 +18488,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2057" r:id="rId210" name="Control 9"/>
+        <control shapeId="2075" r:id="rId210" name="Control 27"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2056" r:id="rId211" name="Control 8">
+        <control shapeId="2076" r:id="rId211" name="Control 28">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>13</xdr:row>
+                <xdr:row>56</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>13</xdr:row>
+                <xdr:row>56</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18623,24 +18513,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2056" r:id="rId211" name="Control 8"/>
+        <control shapeId="2076" r:id="rId211" name="Control 28"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2055" r:id="rId212" name="Control 7">
+        <control shapeId="2077" r:id="rId212" name="Control 29">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
+                <xdr:row>58</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>11</xdr:row>
+                <xdr:row>58</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18648,24 +18538,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2055" r:id="rId212" name="Control 7"/>
+        <control shapeId="2077" r:id="rId212" name="Control 29"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2054" r:id="rId213" name="Control 6">
+        <control shapeId="2078" r:id="rId213" name="Control 30">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>7</xdr:row>
+                <xdr:row>60</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>7</xdr:row>
+                <xdr:row>60</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18673,24 +18563,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2054" r:id="rId213" name="Control 6"/>
+        <control shapeId="2078" r:id="rId213" name="Control 30"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2053" r:id="rId214" name="Control 5">
+        <control shapeId="2079" r:id="rId214" name="Control 31">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>61</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>61</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18698,24 +18588,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2053" r:id="rId214" name="Control 5"/>
+        <control shapeId="2079" r:id="rId214" name="Control 31"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2052" r:id="rId215" name="Control 4">
+        <control shapeId="2080" r:id="rId215" name="Control 32">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>64</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>64</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18723,24 +18613,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2052" r:id="rId215" name="Control 4"/>
+        <control shapeId="2080" r:id="rId215" name="Control 32"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2051" r:id="rId216" name="Control 3">
+        <control shapeId="2081" r:id="rId216" name="Control 33">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>66</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>66</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18748,24 +18638,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2051" r:id="rId216" name="Control 3"/>
+        <control shapeId="2081" r:id="rId216" name="Control 33"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2050" r:id="rId217" name="Control 2">
+        <control shapeId="2082" r:id="rId217" name="Control 34">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>69</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>69</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18773,24 +18663,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2050" r:id="rId217" name="Control 2"/>
+        <control shapeId="2082" r:id="rId217" name="Control 34"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId218" name="Control 1">
+        <control shapeId="2083" r:id="rId218" name="Control 35">
           <controlPr defaultSize="0" r:id="rId184">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
+                <xdr:row>72</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>1</xdr:row>
+                <xdr:row>72</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -18798,7 +18688,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2049" r:id="rId218" name="Control 1"/>
+        <control shapeId="2083" r:id="rId218" name="Control 35"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
All Updated till now, Excepts DSL data and DSL +OLO request
</commit_message>
<xml_diff>
--- a/src/Data/NewOrderStandard.xlsx
+++ b/src/Data/NewOrderStandard.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="405">
   <si>
     <t>Product</t>
   </si>
@@ -1510,12 +1510,6 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>Techincal Contact -Name</t>
-  </si>
-  <si>
-    <t>Techincal Contact Lastname</t>
-  </si>
-  <si>
     <t>Techincal Contact Email</t>
   </si>
   <si>
@@ -1600,9 +1594,6 @@
     <t>End to End journy with Self Approval</t>
   </si>
   <si>
-    <t>Ashwani</t>
-  </si>
-  <si>
     <t>Singh</t>
   </si>
   <si>
@@ -1649,6 +1640,21 @@
   </si>
   <si>
     <t>Renegotiate</t>
+  </si>
+  <si>
+    <t>Offnet Respoence Type</t>
+  </si>
+  <si>
+    <t>Approve</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>Supplier No Bid</t>
+  </si>
+  <si>
+    <t>Nearnet Responce Type</t>
   </si>
 </sst>
 </file>
@@ -7960,8 +7966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7999,7 +8005,7 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -8041,7 +8047,7 @@
         <v>341</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D2" s="34" t="s">
         <v>345</v>
@@ -8053,10 +8059,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I2" s="34" t="s">
         <v>348</v>
@@ -8068,7 +8074,7 @@
         <v>350</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="M2" s="34" t="s">
         <v>351</v>
@@ -8086,106 +8092,106 @@
         <v>355</v>
       </c>
       <c r="R2" s="34" t="s">
+        <v>400</v>
+      </c>
+      <c r="S2" s="34" t="s">
+        <v>404</v>
+      </c>
+      <c r="T2" s="34" t="s">
         <v>356</v>
       </c>
-      <c r="S2" s="34" t="s">
+      <c r="U2" s="34" t="s">
         <v>357</v>
       </c>
-      <c r="T2" s="34" t="s">
+      <c r="V2" s="34" t="s">
         <v>358</v>
       </c>
-      <c r="U2" s="34" t="s">
+      <c r="W2" s="34" t="s">
         <v>359</v>
-      </c>
-      <c r="V2" s="34" t="s">
-        <v>360</v>
-      </c>
-      <c r="W2" s="34" t="s">
-        <v>361</v>
       </c>
       <c r="X2" s="34" t="s">
         <v>344</v>
       </c>
       <c r="Y2" s="34" t="s">
+        <v>379</v>
+      </c>
+      <c r="Z2" s="34" t="s">
+        <v>380</v>
+      </c>
+      <c r="AA2" s="34" t="s">
         <v>381</v>
       </c>
-      <c r="Z2" s="34" t="s">
-        <v>382</v>
-      </c>
-      <c r="AA2" s="34" t="s">
-        <v>383</v>
-      </c>
       <c r="AB2" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="AC2" s="34" t="s">
+        <v>361</v>
+      </c>
+      <c r="AD2" s="34" t="s">
         <v>362</v>
       </c>
-      <c r="AC2" s="34" t="s">
+      <c r="AE2" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="AD2" s="34" t="s">
-        <v>364</v>
-      </c>
-      <c r="AE2" s="34" t="s">
-        <v>365</v>
-      </c>
       <c r="AF2" s="34" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B3" s="44" t="s">
+        <v>390</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>383</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>393</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>396</v>
       </c>
       <c r="E3" s="44">
         <v>267734</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G3" s="36"/>
       <c r="H3" s="36"/>
       <c r="I3" s="33" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="J3" s="33"/>
       <c r="K3" s="33" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L3" s="33"/>
       <c r="M3" s="32" t="s">
         <v>342</v>
       </c>
       <c r="N3" s="32" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="O3" s="36" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="P3" s="32" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="Q3" s="32" t="s">
-        <v>369</v>
-      </c>
-      <c r="R3" s="44" t="s">
+        <v>367</v>
+      </c>
+      <c r="R3" s="39" t="s">
+        <v>403</v>
+      </c>
+      <c r="S3" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="T3" s="47" t="s">
+        <v>385</v>
+      </c>
+      <c r="U3" s="44" t="s">
         <v>386</v>
-      </c>
-      <c r="S3" s="44" t="s">
-        <v>387</v>
-      </c>
-      <c r="T3" s="47" t="s">
-        <v>388</v>
-      </c>
-      <c r="U3" s="44" t="s">
-        <v>389</v>
       </c>
       <c r="V3" s="44">
         <v>123566534</v>
@@ -8194,10 +8200,10 @@
         <v>4534534534</v>
       </c>
       <c r="X3" s="44" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="Y3" s="44" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="Z3" s="44">
         <v>3</v>
@@ -8206,19 +8212,19 @@
         <v>3</v>
       </c>
       <c r="AB3" s="44" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="AC3" s="47" t="s">
+        <v>387</v>
+      </c>
+      <c r="AD3" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="AE3" s="32" t="s">
+        <v>369</v>
+      </c>
+      <c r="AF3" s="32" t="s">
         <v>390</v>
-      </c>
-      <c r="AD3" s="32" t="s">
-        <v>370</v>
-      </c>
-      <c r="AE3" s="32" t="s">
-        <v>371</v>
-      </c>
-      <c r="AF3" s="32" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -8228,34 +8234,36 @@
       <c r="D4" s="44"/>
       <c r="E4" s="44"/>
       <c r="F4" s="36" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
       <c r="I4" s="33" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="J4" s="33"/>
       <c r="K4" s="33" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L4" s="33"/>
       <c r="M4" s="32" t="s">
         <v>342</v>
       </c>
       <c r="N4" s="32" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="O4" s="32" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="P4" s="32" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="Q4" s="32" t="s">
-        <v>369</v>
-      </c>
-      <c r="R4" s="44"/>
+        <v>367</v>
+      </c>
+      <c r="R4" s="39" t="s">
+        <v>402</v>
+      </c>
       <c r="S4" s="44"/>
       <c r="T4" s="47"/>
       <c r="U4" s="44"/>
@@ -8268,27 +8276,27 @@
       <c r="AB4" s="44"/>
       <c r="AC4" s="47"/>
       <c r="AD4" s="32" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AE4" s="32" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AF4" s="32" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="E5" s="38">
         <v>267757</v>
@@ -8299,13 +8307,13 @@
       <c r="G5" s="32"/>
       <c r="H5" s="32"/>
       <c r="I5" s="33" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="K5" s="33" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L5" s="33"/>
       <c r="M5" s="32" t="s">
@@ -8315,23 +8323,23 @@
         <v>343</v>
       </c>
       <c r="O5" s="32" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="P5" s="32" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="Q5" s="32"/>
       <c r="R5" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="S5" s="39" t="s">
+        <v>384</v>
+      </c>
+      <c r="T5" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="U5" s="39" t="s">
         <v>386</v>
-      </c>
-      <c r="S5" s="39" t="s">
-        <v>387</v>
-      </c>
-      <c r="T5" s="40" t="s">
-        <v>388</v>
-      </c>
-      <c r="U5" s="39" t="s">
-        <v>389</v>
       </c>
       <c r="V5" s="39">
         <v>123566534</v>
@@ -8340,29 +8348,29 @@
         <v>4534534534</v>
       </c>
       <c r="X5" s="39" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="Y5" s="39"/>
       <c r="Z5" s="39"/>
       <c r="AA5" s="39"/>
       <c r="AB5" s="39" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="AC5" s="40" t="s">
+        <v>387</v>
+      </c>
+      <c r="AD5" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="AE5" s="32" t="s">
+        <v>369</v>
+      </c>
+      <c r="AF5" s="32" t="s">
         <v>390</v>
       </c>
-      <c r="AD5" s="32" t="s">
-        <v>370</v>
-      </c>
-      <c r="AE5" s="32" t="s">
-        <v>371</v>
-      </c>
-      <c r="AF5" s="32" t="s">
-        <v>393</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="17">
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="W3:W4"/>
     <mergeCell ref="X3:X4"/>
@@ -8376,7 +8384,6 @@
     <mergeCell ref="AA3:AA4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="R3:R4"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="T3:T4"/>
     <mergeCell ref="AC3:AC4"/>
@@ -8482,13 +8489,13 @@
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
       <c r="I3" s="33" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J3" s="32" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="K3" s="33" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L3" s="33"/>
       <c r="M3" s="32" t="s">
@@ -8498,93 +8505,93 @@
         <v>343</v>
       </c>
       <c r="O3" s="32" t="s">
+        <v>366</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q3" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="AD3" s="32" t="s">
         <v>368</v>
       </c>
-      <c r="P3" s="32" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q3" s="32" t="s">
+      <c r="AE3" s="32" t="s">
         <v>369</v>
-      </c>
-      <c r="AD3" s="32" t="s">
-        <v>370</v>
-      </c>
-      <c r="AE3" s="32" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="F4" s="36" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
       <c r="I4" s="33" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J4" s="32"/>
       <c r="K4" s="33" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L4" s="33"/>
       <c r="M4" s="32" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N4" s="37" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="O4" s="36" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="P4" s="32"/>
       <c r="Q4" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="AD4" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="AE4" s="32" t="s">
         <v>369</v>
-      </c>
-      <c r="AD4" s="32" t="s">
-        <v>370</v>
-      </c>
-      <c r="AE4" s="32" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="F5" s="36" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G5" s="36"/>
       <c r="H5" s="36"/>
       <c r="I5" s="33" t="s">
+        <v>364</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>364</v>
+      </c>
+      <c r="K5" s="33" t="s">
+        <v>365</v>
+      </c>
+      <c r="L5" s="33" t="s">
+        <v>376</v>
+      </c>
+      <c r="M5" s="32" t="s">
+        <v>372</v>
+      </c>
+      <c r="N5" s="37" t="s">
+        <v>373</v>
+      </c>
+      <c r="O5" s="36" t="s">
         <v>366</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="P5" s="37" t="s">
         <v>366</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="Q5" s="32" t="s">
         <v>367</v>
       </c>
-      <c r="L5" s="33" t="s">
-        <v>378</v>
-      </c>
-      <c r="M5" s="32" t="s">
-        <v>374</v>
-      </c>
-      <c r="N5" s="37" t="s">
-        <v>375</v>
-      </c>
-      <c r="O5" s="36" t="s">
+      <c r="AD5" s="32" t="s">
         <v>368</v>
       </c>
-      <c r="P5" s="37" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q5" s="32" t="s">
+      <c r="AE5" s="32" t="s">
         <v>369</v>
-      </c>
-      <c r="AD5" s="32" t="s">
-        <v>370</v>
-      </c>
-      <c r="AE5" s="32" t="s">
-        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>